<commit_message>
switched coke cooler over to proper scene kpi setup
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS_SAND/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v8.xlsx
+++ b/Projects/CCBOTTLERSUS_SAND/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v8.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="136">
   <si>
     <t xml:space="preserve">KPI name</t>
   </si>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">program (Additional Attribute 3)</t>
   </si>
   <si>
-    <t xml:space="preserve">scene level</t>
+    <t xml:space="preserve">session_level</t>
   </si>
   <si>
     <t xml:space="preserve">Sparkling</t>
@@ -65,6 +65,9 @@
     <t xml:space="preserve">Club Coke Chill Plus,Club Coke Chill,Club Coke Gold,Club Coke Silver,NTBA</t>
   </si>
   <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">Still</t>
   </si>
   <si>
@@ -174,9 +177,6 @@
   </si>
   <si>
     <t xml:space="preserve">Coke Cooler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
   </si>
   <si>
     <t xml:space="preserve">Param 1</t>
@@ -978,18 +978,18 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="51:51 A16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.1295546558705"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.663967611336"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -1032,10 +1032,13 @@
       <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1047,12 +1050,15 @@
         <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1064,12 +1070,15 @@
         <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -1081,15 +1090,18 @@
         <v>10</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
@@ -1098,15 +1110,18 @@
         <v>10</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
@@ -1115,15 +1130,18 @@
         <v>10</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
@@ -1132,15 +1150,18 @@
         <v>10</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>9</v>
@@ -1149,15 +1170,18 @@
         <v>10</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>9</v>
@@ -1166,15 +1190,18 @@
         <v>10</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>9</v>
@@ -1183,30 +1210,36 @@
         <v>10</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
@@ -1218,12 +1251,15 @@
         <v>10</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>8</v>
@@ -1235,12 +1271,15 @@
         <v>10</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
@@ -1252,12 +1291,15 @@
         <v>10</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
@@ -1269,12 +1311,15 @@
         <v>10</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
@@ -1286,176 +1331,203 @@
         <v>10</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="0" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1478,7 +1550,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="51:51 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1507,13 +1579,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1535,13 +1607,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="51:51 B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="7" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="46.4898785425101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="46.8097165991903"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="7" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="8" width="9.21052631578947"/>
@@ -1589,22 +1661,22 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="1" sqref="51:51 A22"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="46.4898785425101"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="46.4898785425101"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="46.8097165991903"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="46.8097165991903"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.21052631578947"/>
   </cols>
@@ -1661,7 +1733,7 @@
         <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>71</v>
@@ -1675,33 +1747,33 @@
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>74</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>74</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>75</v>
@@ -1713,7 +1785,7 @@
         <v>54</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>71</v>
@@ -1722,12 +1794,12 @@
         <v>77</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>75</v>
@@ -1739,7 +1811,7 @@
         <v>54</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>71</v>
@@ -1748,58 +1820,58 @@
         <v>77</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>71</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>71</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>71</v>
@@ -1811,7 +1883,7 @@
         <v>54</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>71</v>
@@ -1822,7 +1894,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>80</v>
@@ -1834,36 +1906,36 @@
         <v>54</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>71</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>71</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1885,16 +1957,16 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="1" sqref="51:51 I8"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5668016194332"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21052631578947"/>
   </cols>
@@ -1927,7 +1999,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
@@ -1945,12 +2017,12 @@
         <v>54</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>80</v>
@@ -1962,18 +2034,18 @@
         <v>54</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>88</v>
@@ -1985,12 +2057,12 @@
         <v>54</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>75</v>
@@ -2002,15 +2074,15 @@
         <v>54</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>75</v>
@@ -2028,12 +2100,12 @@
         <v>54</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>75</v>
@@ -2045,7 +2117,7 @@
         <v>54</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2067,12 +2139,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="51:51 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.21052631578947"/>
   </cols>
@@ -2096,13 +2168,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2123,17 +2195,17 @@
   </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="51:51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="38.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
@@ -2176,7 +2248,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>98</v>
@@ -2193,7 +2265,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>98</v>
@@ -2210,7 +2282,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>98</v>
@@ -2227,7 +2299,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>100</v>
@@ -2244,7 +2316,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>100</v>
@@ -2261,7 +2333,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>100</v>
@@ -2278,7 +2350,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>104</v>
@@ -2295,7 +2367,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>104</v>
@@ -2312,7 +2384,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>104</v>
@@ -2329,7 +2401,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>108</v>
@@ -2363,7 +2435,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>98</v>
@@ -2380,7 +2452,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>98</v>
@@ -2397,7 +2469,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>98</v>
@@ -2414,7 +2486,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>100</v>
@@ -2431,7 +2503,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>100</v>
@@ -2448,7 +2520,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>100</v>
@@ -2465,7 +2537,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>104</v>
@@ -2482,7 +2554,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>104</v>
@@ -2499,7 +2571,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>104</v>
@@ -2516,7 +2588,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>108</v>
@@ -2550,7 +2622,7 @@
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>98</v>
@@ -2567,7 +2639,7 @@
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>98</v>
@@ -2584,7 +2656,7 @@
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>98</v>
@@ -2601,7 +2673,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>100</v>
@@ -2618,7 +2690,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>100</v>
@@ -2635,7 +2707,7 @@
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>100</v>
@@ -2652,7 +2724,7 @@
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>104</v>
@@ -2669,7 +2741,7 @@
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>104</v>
@@ -2686,7 +2758,7 @@
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>104</v>
@@ -2703,7 +2775,7 @@
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>108</v>
@@ -2737,7 +2809,7 @@
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>98</v>
@@ -2754,7 +2826,7 @@
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>98</v>
@@ -2771,7 +2843,7 @@
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>98</v>
@@ -2788,7 +2860,7 @@
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>100</v>
@@ -2805,7 +2877,7 @@
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>100</v>
@@ -2822,7 +2894,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>100</v>
@@ -2839,7 +2911,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>104</v>
@@ -2856,7 +2928,7 @@
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>104</v>
@@ -2873,7 +2945,7 @@
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>104</v>
@@ -2890,7 +2962,7 @@
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>108</v>
@@ -2916,7 +2988,7 @@
         <v>96</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F46" s="29" t="n">
         <v>0.38</v>
@@ -2924,7 +2996,7 @@
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>104</v>
@@ -2933,7 +3005,7 @@
         <v>96</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F47" s="29" t="n">
         <v>0.15</v>
@@ -2941,7 +3013,7 @@
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>95</v>
@@ -2950,7 +3022,7 @@
         <v>96</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F48" s="30" t="n">
         <v>0.3</v>
@@ -2958,7 +3030,7 @@
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>95</v>
@@ -2967,7 +3039,7 @@
         <v>96</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F49" s="30" t="n">
         <v>0.33</v>
@@ -2975,7 +3047,7 @@
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>95</v>
@@ -2984,7 +3056,7 @@
         <v>96</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F50" s="30" t="n">
         <v>0.15</v>
@@ -2992,7 +3064,7 @@
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>95</v>
@@ -3001,7 +3073,7 @@
         <v>96</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F51" s="30" t="n">
         <v>0.5</v>
@@ -3009,7 +3081,7 @@
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>95</v>
@@ -3018,7 +3090,7 @@
         <v>96</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F52" s="30" t="n">
         <v>0.2</v>
@@ -3043,17 +3115,17 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="51:51 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.6356275303644"/>
     <col collapsed="false" hidden="false" max="14" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.46153846153846"/>
   </cols>
@@ -3104,7 +3176,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>75</v>
@@ -3119,7 +3191,7 @@
         <v>126</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G2" s="35" t="n">
         <v>2</v>
@@ -3136,7 +3208,7 @@
     </row>
     <row r="3" customFormat="false" ht="48.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>127</v>
@@ -3145,7 +3217,7 @@
         <v>128</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G3" s="39" t="n">
         <v>2</v>
@@ -3162,7 +3234,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>75</v>
@@ -3171,7 +3243,7 @@
         <v>129</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4" s="39"/>
       <c r="H4" s="40"/>
@@ -3196,7 +3268,7 @@
     </row>
     <row r="5" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>127</v>
@@ -3207,7 +3279,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="14"/>
       <c r="F5" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5" s="39"/>
       <c r="H5" s="40"/>
@@ -3232,7 +3304,7 @@
     </row>
     <row r="6" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>127</v>
@@ -3241,7 +3313,7 @@
         <v>131</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G6" s="39"/>
       <c r="H6" s="40"/>
@@ -3271,7 +3343,7 @@
         <v>132</v>
       </c>
       <c r="F7" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G7" s="39"/>
       <c r="H7" s="40"/>
@@ -3296,7 +3368,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>75</v>
@@ -3305,7 +3377,7 @@
         <v>133</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G8" s="39"/>
       <c r="H8" s="40"/>
@@ -3330,7 +3402,7 @@
     </row>
     <row r="9" customFormat="false" ht="82.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>127</v>
@@ -3339,7 +3411,7 @@
         <v>134</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G9" s="43"/>
       <c r="H9" s="44"/>
@@ -3364,7 +3436,7 @@
     </row>
     <row r="10" customFormat="false" ht="48.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>127</v>
@@ -3373,7 +3445,7 @@
         <v>135</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
changed num & den param pulling fixed category issue with template fixed impulse zone target display moved shelves bonus back under shelves and    silenced it's results.
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS_SAND/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v8.xlsx
+++ b/Projects/CCBOTTLERSUS_SAND/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v8.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="137">
   <si>
     <t xml:space="preserve">KPI name</t>
   </si>
@@ -981,18 +981,18 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3:H27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.663967611336"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="66.1983805668016"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -1634,7 +1634,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H3:H27 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1691,13 +1691,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="H3:H27 B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="7" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="46.8097165991903"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="47.1336032388664"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="7" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="8" width="9.21052631578947"/>
@@ -1745,22 +1745,22 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="1" sqref="H3:H27 A22"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="46.8097165991903"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="46.8097165991903"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.919028340081"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.21052631578947"/>
   </cols>
@@ -1855,7 +1855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
         <v>17</v>
       </c>
@@ -1870,6 +1870,12 @@
       </c>
       <c r="E4" s="16" t="s">
         <v>13</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>79</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>73</v>
@@ -1897,6 +1903,12 @@
       <c r="E5" s="16" t="s">
         <v>13</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="H5" s="1" t="s">
         <v>73</v>
       </c>
@@ -1991,6 +2003,12 @@
       </c>
       <c r="E9" s="16" t="s">
         <v>13</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>73</v>
@@ -2041,16 +2059,16 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="1" sqref="H3:H27 I8"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.7813765182186"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21052631578947"/>
   </cols>
@@ -2223,12 +2241,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H3:H27 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.21052631578947"/>
   </cols>
@@ -2279,17 +2297,17 @@
   </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A51" activeCellId="1" sqref="H3:H27 A51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="38.668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
@@ -3199,17 +3217,17 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H3:H27 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.919028340081"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="14" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.46153846153846"/>
   </cols>

</xml_diff>

<commit_message>
adding functionality to scene session
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS_SAND/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v8.xlsx
+++ b/Projects/CCBOTTLERSUS_SAND/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v8.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="137">
   <si>
     <t xml:space="preserve">KPI name</t>
   </si>
@@ -981,17 +981,17 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="66.1983805668016"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="66.8421052631579"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21052631578947"/>
   </cols>
@@ -1391,7 +1391,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>37</v>
       </c>
@@ -1407,14 +1407,11 @@
       <c r="F18" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="H18" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>40</v>
       </c>
@@ -1430,14 +1427,11 @@
       <c r="F19" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="H19" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>41</v>
       </c>
@@ -1453,14 +1447,11 @@
       <c r="F20" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="H20" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>42</v>
       </c>
@@ -1476,14 +1467,11 @@
       <c r="F21" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="H21" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>43</v>
       </c>
@@ -1499,14 +1487,11 @@
       <c r="F22" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="H22" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>44</v>
       </c>
@@ -1522,14 +1507,11 @@
       <c r="F23" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="H23" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>45</v>
       </c>
@@ -1545,14 +1527,11 @@
       <c r="F24" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="H24" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>46</v>
       </c>
@@ -1568,14 +1547,11 @@
       <c r="F25" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G25" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="H25" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -1590,9 +1566,6 @@
       </c>
       <c r="F26" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>14</v>
@@ -1697,7 +1670,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="7" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="7" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="8" width="9.21052631578947"/>
@@ -1750,17 +1723,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="47.1336032388664"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.1336032388664"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.2429149797571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="47.4534412955466"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.4534412955466"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.21052631578947"/>
   </cols>
@@ -2064,11 +2037,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21052631578947"/>
   </cols>
@@ -2246,7 +2219,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.21052631578947"/>
   </cols>
@@ -2297,17 +2270,17 @@
   </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="38.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
@@ -3222,12 +3195,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="14" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.46153846153846"/>
   </cols>

</xml_diff>

<commit_message>
updated template for impulse zone cooler
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS_SAND/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v8.xlsx
+++ b/Projects/CCBOTTLERSUS_SAND/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v8.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="137">
   <si>
     <t xml:space="preserve">KPI name</t>
   </si>
@@ -981,17 +981,17 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="66.8421052631579"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="67.4858299595142"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21052631578947"/>
   </cols>
@@ -1252,7 +1252,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -1268,9 +1268,6 @@
       <c r="E12" s="3"/>
       <c r="F12" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>14</v>
@@ -1670,7 +1667,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="7" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="47.4534412955466"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="47.8825910931174"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="7" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="8" width="9.21052631578947"/>
@@ -1723,17 +1720,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="47.4534412955466"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.4534412955466"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.5627530364372"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="47.8825910931174"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.8825910931174"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.21052631578947"/>
   </cols>
@@ -2032,16 +2029,16 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2064777327935"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21052631578947"/>
   </cols>
@@ -2219,7 +2216,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.21052631578947"/>
   </cols>
@@ -2276,11 +2273,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="39.3117408906883"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
@@ -3190,17 +3187,17 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.4939271255061"/>
     <col collapsed="false" hidden="false" max="14" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.46153846153846"/>
   </cols>

</xml_diff>

<commit_message>
made nice with mobile reports
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS_SAND/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v8.xlsx
+++ b/Projects/CCBOTTLERSUS_SAND/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v8.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="137">
   <si>
     <t xml:space="preserve">KPI name</t>
   </si>
@@ -981,17 +981,17 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="67.4858299595142"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="68.0202429149798"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21052631578947"/>
   </cols>
@@ -1268,6 +1268,9 @@
       <c r="E12" s="3"/>
       <c r="F12" s="0" t="s">
         <v>16</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>14</v>
@@ -1667,7 +1670,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="7" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="47.8825910931174"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="48.3117408906883"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="7" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="8" width="9.21052631578947"/>
@@ -1720,17 +1723,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="47.8825910931174"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.8825910931174"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.8825910931174"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="48.3117408906883"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="48.3117408906883"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.21052631578947"/>
   </cols>
@@ -2034,11 +2037,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21052631578947"/>
   </cols>
@@ -2216,7 +2219,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.21052631578947"/>
   </cols>
@@ -2273,11 +2276,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="39.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
@@ -3192,12 +3195,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9919028340081"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3481781376518"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="14" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.46153846153846"/>
   </cols>

</xml_diff>